<commit_message>
Updated LEDs and part numbers
</commit_message>
<xml_diff>
--- a/T41_DXL/T41 DXL XBEE PCS BOM.xlsx
+++ b/T41_DXL/T41 DXL XBEE PCS BOM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Teensy3.1-Breakout-Boards\T41_DXL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F35315-C15D-461A-B925-4E99AB09A8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540"/>
+    <workbookView xWindow="11130" yWindow="5040" windowWidth="27675" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>Item #</t>
   </si>
@@ -116,9 +122,6 @@
     </r>
   </si>
   <si>
-    <t>BT1</t>
-  </si>
-  <si>
     <t>C1, C3, C6, C7, C8, C10</t>
   </si>
   <si>
@@ -149,21 +152,6 @@
     <t>THT</t>
   </si>
   <si>
-    <t>JAX1, JAX2, JAX3, JAX4, JAX5, JAX-PWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOLEX </t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 3POS 2.5MM THT</t>
-  </si>
-  <si>
-    <t>L31, L32, RSSI, RX, TX</t>
-  </si>
-  <si>
-    <t>LED YELLOW 805</t>
-  </si>
-  <si>
     <t>TRANSISTOR T2222</t>
   </si>
   <si>
@@ -257,33 +245,12 @@
     <t>JQW</t>
   </si>
   <si>
-    <t>Qwiic JST Connector - SMD 4-pin(Vertical)</t>
-  </si>
-  <si>
     <t>JQW1, JQW2</t>
   </si>
   <si>
-    <t>Qwiic JST Connector - SMD 4-pin(Horizontal)</t>
-  </si>
-  <si>
     <t>DIODE ZENER 15V 500MW SOD123</t>
   </si>
   <si>
-    <t xml:space="preserve"> Seiko Instruments</t>
-  </si>
-  <si>
-    <t>ML414H IV01E</t>
-  </si>
-  <si>
-    <t>BATTERY LITHIUM 3V RECHARGE</t>
-  </si>
-  <si>
-    <t>2Pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IC REG LINEAR 3.3V 250MA SOT89-3</t>
-  </si>
-  <si>
     <t>SOT89-3</t>
   </si>
   <si>
@@ -293,9 +260,6 @@
     <t>292303-1</t>
   </si>
   <si>
-    <t>BIOLOID-MOLEX_JST</t>
-  </si>
-  <si>
     <t>JST04_1MM_RA</t>
   </si>
   <si>
@@ -303,18 +267,103 @@
   </si>
   <si>
     <t>CHIPLED_0805</t>
+  </si>
+  <si>
+    <t>LED Green 805</t>
+  </si>
+  <si>
+    <t>LED Red 805</t>
+  </si>
+  <si>
+    <t>L31, RSSI, RX</t>
+  </si>
+  <si>
+    <t>L32,TX</t>
+  </si>
+  <si>
+    <t>Infineon Technologies</t>
+  </si>
+  <si>
+    <t>BAT60AE6327HTSA1</t>
+  </si>
+  <si>
+    <t>LSM115JE3/TR13</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>74LVC1G126GV,125</t>
+  </si>
+  <si>
+    <t>Nexperia USA Inc</t>
+  </si>
+  <si>
+    <t>74HC1G125GV,125</t>
+  </si>
+  <si>
+    <t>SUP90P06-09L-E3</t>
+  </si>
+  <si>
+    <t>Vichay Siliconix</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>ON Semicondutor</t>
+  </si>
+  <si>
+    <t>MMBT6428</t>
+  </si>
+  <si>
+    <t>Firchild Semicondutor</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>BZT52C15-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IC REG LINEAR 3.3V 600MA SOT89-3</t>
+  </si>
+  <si>
+    <t>AP7365-33YG-13</t>
+  </si>
+  <si>
+    <t>JST Sales</t>
+  </si>
+  <si>
+    <t>Qwiic JST SH 1mm Connector - SMD 4-pin(Vertical)</t>
+  </si>
+  <si>
+    <t>Qwiic JST SH 1mm Connector - SMD 4-pin(Horizontal)</t>
+  </si>
+  <si>
+    <t>BM04B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM04B-SRSS-TB(LF)(SN)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -419,23 +468,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -445,33 +494,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,6 +525,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -504,7 +550,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="pcbway-400x400.jpg"/>
+        <xdr:cNvPr id="2" name="图片 1" descr="pcbway-400x400.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -814,11 +866,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G27"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -826,34 +878,34 @@
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="42.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="D2" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="D2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -881,46 +933,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="15">
       <c r="A7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="15">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="8">
+        <v>805</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6">
         <v>2</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6">
-        <v>6</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="8">
         <v>805</v>
@@ -931,18 +979,18 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="8">
         <v>805</v>
@@ -953,18 +1001,18 @@
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="8" t="s">
-        <v>13</v>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="G10" s="8">
         <v>805</v>
@@ -975,135 +1023,143 @@
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="A11" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="6">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
       <c r="F11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="8">
-        <v>805</v>
-      </c>
-      <c r="H11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="10" t="s">
-        <v>61</v>
+      <c r="F12" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C13" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15">
       <c r="A14" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="15">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="H15" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="8">
-        <v>22035035</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15">
-      <c r="A15" s="6">
-        <v>11</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="6">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="15">
-      <c r="A16" s="6">
-        <v>13</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>4</v>
@@ -1111,21 +1167,25 @@
     </row>
     <row r="17" spans="1:8" ht="15">
       <c r="A17" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6">
-        <v>3</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
       <c r="F17" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>4</v>
@@ -1133,21 +1193,21 @@
     </row>
     <row r="18" spans="1:8" ht="15">
       <c r="A18" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>34</v>
+      <c r="F18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="9">
+        <v>805</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>4</v>
@@ -1155,18 +1215,18 @@
     </row>
     <row r="19" spans="1:8" ht="15">
       <c r="A19" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G19" s="9">
         <v>805</v>
@@ -1177,18 +1237,18 @@
     </row>
     <row r="20" spans="1:8" ht="15">
       <c r="A20" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G20" s="9">
         <v>805</v>
@@ -1199,18 +1259,18 @@
     </row>
     <row r="21" spans="1:8" ht="15">
       <c r="A21" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C21" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G21" s="9">
         <v>805</v>
@@ -1221,18 +1281,18 @@
     </row>
     <row r="22" spans="1:8" ht="15">
       <c r="A22" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C22" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G22" s="9">
         <v>805</v>
@@ -1243,10 +1303,10 @@
     </row>
     <row r="23" spans="1:8" ht="15">
       <c r="A23" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -1254,7 +1314,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G23" s="9">
         <v>805</v>
@@ -1263,67 +1323,79 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8" ht="17.25" customHeight="1">
       <c r="A24" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="9">
-        <v>805</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17.25" customHeight="1">
+      <c r="D24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="6">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="10" t="s">
+      <c r="D25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15">
       <c r="A26" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
+      </c>
       <c r="F26" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>4</v>
@@ -1331,21 +1403,25 @@
     </row>
     <row r="27" spans="1:8" ht="15">
       <c r="A27" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
       <c r="F27" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>4</v>
@@ -1353,21 +1429,25 @@
     </row>
     <row r="28" spans="1:8" ht="15">
       <c r="A28" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
       <c r="F28" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>4</v>
@@ -1375,21 +1455,25 @@
     </row>
     <row r="29" spans="1:8" ht="15">
       <c r="A29" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F29" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>54</v>
+        <v>82</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>4</v>
@@ -1397,45 +1481,27 @@
     </row>
     <row r="30" spans="1:8" ht="15">
       <c r="A30" s="6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="6">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="6">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="H30" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15">
-      <c r="A31" s="6">
-        <v>32</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="6">
-        <v>2</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H31" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1451,7 +1517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1464,7 +1530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>